<commit_message>
feat: add prepro and traffic parameters
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12080"/>
+    <workbookView windowWidth="28800" windowHeight="12280"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -27,33 +27,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+  <si>
+    <t>参数类别</t>
+  </si>
+  <si>
+    <t>参数名称</t>
+  </si>
+  <si>
+    <t>符号</t>
+  </si>
+  <si>
+    <t>数值</t>
+  </si>
   <si>
     <t>标定参数</t>
   </si>
   <si>
-    <t>内侧道路元胞分割距离d_cell(m)</t>
+    <t>内侧道路元胞分割距离</t>
+  </si>
+  <si>
+    <t>d_cell(m)</t>
   </si>
   <si>
     <t>50m</t>
   </si>
   <si>
-    <t>合流元胞判定交通量q_merge(v/h)</t>
+    <t>合流元胞判定交通量</t>
+  </si>
+  <si>
+    <t>q_merge(v/h)</t>
+  </si>
+  <si>
+    <t>事件检测参数</t>
   </si>
   <si>
     <t>共用参数</t>
   </si>
   <si>
-    <t>帧率FPS</t>
-  </si>
-  <si>
-    <t>低速判定速度v_low(m/s)</t>
+    <t>帧率</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>低速判定速度</t>
+  </si>
+  <si>
+    <t>v_low(m/s)</t>
   </si>
   <si>
     <t>10/3.6 = 2.778m/s</t>
   </si>
   <si>
-    <t>高速判定速度v_high(m/s)</t>
+    <t>高速判定速度</t>
+  </si>
+  <si>
+    <t>v_high(m/s)</t>
   </si>
   <si>
     <t>120/3.6 = 33.33m/s</t>
@@ -62,25 +92,37 @@
     <t>抛洒物检测</t>
   </si>
   <si>
-    <t>抛洒物处理容忍时间t_tolerance(s)</t>
+    <t>抛洒物处理容忍时间</t>
+  </si>
+  <si>
+    <t>t_tolerance(s)</t>
   </si>
   <si>
     <t>300s</t>
   </si>
   <si>
-    <t>抛洒物置信度时间增长率rate1(/frame)</t>
+    <t>抛洒物置信度时间增长率</t>
+  </si>
+  <si>
+    <t>rate1(/frame)</t>
   </si>
   <si>
     <t>1/(t_tolerance *FPS)</t>
   </si>
   <si>
-    <t>抛洒物置信度换道增长率rate2(1)</t>
+    <t>抛洒物置信度换道增长率</t>
+  </si>
+  <si>
+    <t>rate2(1)</t>
   </si>
   <si>
     <t>事故检测</t>
   </si>
   <si>
-    <t>接触距离d_touch(m)</t>
+    <t>接触距离</t>
+  </si>
+  <si>
+    <t>d_touch(m)</t>
   </si>
   <si>
     <t>5m(两车追尾距离等于1个车长)</t>
@@ -89,22 +131,19 @@
     <t>拥堵检测</t>
   </si>
   <si>
-    <t>拥堵密度density_crowd(/m)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>18pcu/km/ln</t>
-    </r>
-  </si>
-  <si>
-    <t>拥堵速度v_crowd(/m)</t>
+    <t>拥堵密度</t>
+  </si>
+  <si>
+    <t>density_crowd(pcu/km/ln)</t>
+  </si>
+  <si>
+    <t>18pcu/km/ln</t>
+  </si>
+  <si>
+    <t>拥堵速度</t>
+  </si>
+  <si>
+    <t>v_crowd(m/s)</t>
   </si>
   <si>
     <t>16.67m/s</t>
@@ -113,13 +152,19 @@
     <t>异常急刹</t>
   </si>
   <si>
-    <t>急刹加速度a_intense(m/s^2)</t>
+    <t>急刹加速度</t>
+  </si>
+  <si>
+    <t>a_intense(m/s^2)</t>
   </si>
   <si>
     <t>3m/s^2</t>
   </si>
   <si>
-    <t>急刹持续时间duration_intense(s)</t>
+    <t>急刹持续时间</t>
+  </si>
+  <si>
+    <t>duration_intense(s)</t>
   </si>
   <si>
     <t>1s</t>
@@ -128,7 +173,10 @@
     <t>停车/应急车道占用</t>
   </si>
   <si>
-    <t>低速持续时间duration_low(s)</t>
+    <t>低速持续时间</t>
+  </si>
+  <si>
+    <t>duration_low(s)</t>
   </si>
   <si>
     <t>5s</t>
@@ -137,7 +185,55 @@
     <t>超速行驶</t>
   </si>
   <si>
-    <t>超速持续时间duration_high(s)</t>
+    <t>超速持续时间</t>
+  </si>
+  <si>
+    <t>duration_high(s)</t>
+  </si>
+  <si>
+    <t>交通流计算参数</t>
+  </si>
+  <si>
+    <t>流量计算</t>
+  </si>
+  <si>
+    <t>交通量计算采样时间</t>
+  </si>
+  <si>
+    <t>q_cal_duration(s)</t>
+  </si>
+  <si>
+    <t>参数更新</t>
+  </si>
+  <si>
+    <t>计算间隔时间</t>
+  </si>
+  <si>
+    <t>cal_interval(s)</t>
+  </si>
+  <si>
+    <t>1/FPS(就每帧都计算)</t>
+  </si>
+  <si>
+    <t>预处理参数</t>
+  </si>
+  <si>
+    <t>轨迹补全</t>
+  </si>
+  <si>
+    <t>最大补全帧数</t>
+  </si>
+  <si>
+    <t>max_complete_frames</t>
+  </si>
+  <si>
+    <t>轨迹平滑</t>
+  </si>
+  <si>
+    <t>平滑指数</t>
+  </si>
+  <si>
+    <t>smooth_alpha</t>
   </si>
 </sst>
 </file>
@@ -151,9 +247,24 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -632,147 +743,150 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1311,178 +1425,327 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="19.6363636363636" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.9090909090909" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.6363636363636" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.81818181818182" style="1"/>
+    <col min="1" max="1" width="14.6363636363636" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.6363636363636" style="2" customWidth="1"/>
+    <col min="3" max="4" width="39.9090909090909" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.6363636363636" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.81818181818182" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" ht="17.5" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4">
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="2">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: set vaule of params of prepro & traffic cal
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12280"/>
+    <workbookView windowWidth="25600" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
     <t>cal_interval(s)</t>
   </si>
   <si>
-    <t>1/FPS(就每帧都计算)</t>
+    <t>30s</t>
   </si>
   <si>
     <t>预处理参数</t>
@@ -1428,7 +1428,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
docs: add a parameter
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>参数类别</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>300s</t>
+  </si>
+  <si>
+    <t>道路设计标准流量参考值</t>
+  </si>
+  <si>
+    <t>q_standard(v/h)</t>
   </si>
   <si>
     <t>抛洒物置信度时间增长率</t>
@@ -1425,10 +1431,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1552,185 +1558,198 @@
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
+      <c r="E8" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>32</v>
+      <c r="E10" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="2" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="2">
+      <c r="C20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="2" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="2">
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="2">
         <v>0.1</v>
       </c>
     </row>
@@ -1738,14 +1757,14 @@
   <mergeCells count="10">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A4:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
fix: add new config parameters
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>参数类别</t>
   </si>
@@ -59,6 +59,24 @@
     <t>q_merge(v/h)</t>
   </si>
   <si>
+    <t>普通车道宽度</t>
+  </si>
+  <si>
+    <t>lane_width(m)</t>
+  </si>
+  <si>
+    <t>3.75m</t>
+  </si>
+  <si>
+    <t>应急车道宽度</t>
+  </si>
+  <si>
+    <t>emgc_width(m)</t>
+  </si>
+  <si>
+    <t>3.5m</t>
+  </si>
+  <si>
     <t>事件检测参数</t>
   </si>
   <si>
@@ -89,6 +107,24 @@
     <t>120/3.6 = 33.33m/s</t>
   </si>
   <si>
+    <t>准静止判定速度</t>
+  </si>
+  <si>
+    <t>v_static(m/s)</t>
+  </si>
+  <si>
+    <t>40/3.6 = 11.11m/s</t>
+  </si>
+  <si>
+    <t>事件类别</t>
+  </si>
+  <si>
+    <t>event_types</t>
+  </si>
+  <si>
+    <t>["crowd", "high_speed", "illegal_occupation", "incident_single_car", "incident", "intensive_speed_reduction", "low_speed", "spill"]</t>
+  </si>
+  <si>
     <t>抛洒物检测</t>
   </si>
   <si>
@@ -107,6 +143,9 @@
     <t>q_standard(v/h)</t>
   </si>
   <si>
+    <t>10000v/h</t>
+  </si>
+  <si>
     <t>抛洒物置信度时间增长率</t>
   </si>
   <si>
@@ -176,25 +215,43 @@
     <t>1s</t>
   </si>
   <si>
-    <t>停车/应急车道占用</t>
+    <t>应急车道占用</t>
+  </si>
+  <si>
+    <t>占用持续时间</t>
+  </si>
+  <si>
+    <t>duration_occupation(s)</t>
+  </si>
+  <si>
+    <t>5s</t>
+  </si>
+  <si>
+    <t>停车</t>
+  </si>
+  <si>
+    <t>准静止持续时间</t>
+  </si>
+  <si>
+    <t>duration_static(s)</t>
+  </si>
+  <si>
+    <t>超速行驶</t>
+  </si>
+  <si>
+    <t>超速持续时间</t>
+  </si>
+  <si>
+    <t>duration_high(s)</t>
+  </si>
+  <si>
+    <t>低速行驶</t>
   </si>
   <si>
     <t>低速持续时间</t>
   </si>
   <si>
     <t>duration_low(s)</t>
-  </si>
-  <si>
-    <t>5s</t>
-  </si>
-  <si>
-    <t>超速行驶</t>
-  </si>
-  <si>
-    <t>超速持续时间</t>
-  </si>
-  <si>
-    <t>duration_high(s)</t>
   </si>
   <si>
     <t>交通流计算参数</t>
@@ -253,7 +310,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +342,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.25"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -623,12 +687,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -749,137 +828,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -889,13 +968,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1431,10 +1519,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1468,303 +1556,385 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>19</v>
+      </c>
+      <c r="E6" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="2">
-        <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" ht="70" spans="1:5">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="5">
-        <v>0.1</v>
+      <c r="E10" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>45</v>
+      <c r="E14" s="8">
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4"/>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="C20" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="E20" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="2">
+      <c r="D22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="5">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
doc: update params of event detect
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
   <si>
     <t>参数类别</t>
   </si>
@@ -41,13 +41,37 @@
     <t>数值</t>
   </si>
   <si>
+    <t>基础参数</t>
+  </si>
+  <si>
+    <t>帧率</t>
+  </si>
+  <si>
+    <t>fps</t>
+  </si>
+  <si>
     <t>标定参数</t>
   </si>
   <si>
-    <t>内侧道路元胞分割距离</t>
-  </si>
-  <si>
-    <t>d_cell(m)</t>
+    <t>是否重新标定(在clb存在情况下是否重来)</t>
+  </si>
+  <si>
+    <t>if_recalib</t>
+  </si>
+  <si>
+    <t>标定过程持续时间</t>
+  </si>
+  <si>
+    <t>calib_seconds(s)</t>
+  </si>
+  <si>
+    <t>600s</t>
+  </si>
+  <si>
+    <t>元胞分割距离</t>
+  </si>
+  <si>
+    <t>cell_len(m)</t>
   </si>
   <si>
     <t>50m</t>
@@ -77,16 +101,121 @@
     <t>3.5m</t>
   </si>
   <si>
-    <t>事件检测参数</t>
-  </si>
-  <si>
-    <t>共用参数</t>
-  </si>
-  <si>
-    <t>帧率</t>
-  </si>
-  <si>
-    <t>FPS</t>
+    <t>交通流计算参数</t>
+  </si>
+  <si>
+    <t>流量计算</t>
+  </si>
+  <si>
+    <t>交通量计算采样时间</t>
+  </si>
+  <si>
+    <t>q_cal_duration(s)</t>
+  </si>
+  <si>
+    <t>300s</t>
+  </si>
+  <si>
+    <t>参数更新</t>
+  </si>
+  <si>
+    <t>计算间隔时间</t>
+  </si>
+  <si>
+    <t>cal_interval(s)</t>
+  </si>
+  <si>
+    <t>30s</t>
+  </si>
+  <si>
+    <t>预处理参数</t>
+  </si>
+  <si>
+    <t>轨迹补全</t>
+  </si>
+  <si>
+    <t>最大补全帧数</t>
+  </si>
+  <si>
+    <t>max_complete_frames</t>
+  </si>
+  <si>
+    <t>轨迹平滑</t>
+  </si>
+  <si>
+    <t>平滑指数</t>
+  </si>
+  <si>
+    <t>smooth_alpha</t>
+  </si>
+  <si>
+    <t>事件检测</t>
+  </si>
+  <si>
+    <t>事件类别</t>
+  </si>
+  <si>
+    <t>event_types</t>
+  </si>
+  <si>
+    <t>['spill','stop', 'low_speed', 'high_speed', 'emergency_break', 'incident', 'crowd', 'illegal_occupation']</t>
+  </si>
+  <si>
+    <t>抛洒物检测</t>
+  </si>
+  <si>
+    <t>抛洒物处理容忍时间</t>
+  </si>
+  <si>
+    <t>t_tolerance(s)</t>
+  </si>
+  <si>
+    <t>道路设计标准流量参考值</t>
+  </si>
+  <si>
+    <t>q_standard(v/h)</t>
+  </si>
+  <si>
+    <t>10000v/h</t>
+  </si>
+  <si>
+    <t>抛洒物置信度时间增长率</t>
+  </si>
+  <si>
+    <t>rate1(/frame)</t>
+  </si>
+  <si>
+    <t>1/(t_tolerance *FPS)</t>
+  </si>
+  <si>
+    <t>抛洒物置信度换道增长率</t>
+  </si>
+  <si>
+    <t>rate2(1)</t>
+  </si>
+  <si>
+    <t>停车</t>
+  </si>
+  <si>
+    <t>准静止判定速度</t>
+  </si>
+  <si>
+    <t>v_static(m/s)</t>
+  </si>
+  <si>
+    <t>3.6/3.6 = 1m/s</t>
+  </si>
+  <si>
+    <t>准静止持续时间</t>
+  </si>
+  <si>
+    <t>duration_static(s)</t>
+  </si>
+  <si>
+    <t>5s</t>
+  </si>
+  <si>
+    <t>低速行驶</t>
   </si>
   <si>
     <t>低速判定速度</t>
@@ -98,6 +227,15 @@
     <t>10/3.6 = 2.778m/s</t>
   </si>
   <si>
+    <t>低速持续时间</t>
+  </si>
+  <si>
+    <t>duration_low(s)</t>
+  </si>
+  <si>
+    <t>超速行驶</t>
+  </si>
+  <si>
     <t>高速判定速度</t>
   </si>
   <si>
@@ -107,58 +245,31 @@
     <t>120/3.6 = 33.33m/s</t>
   </si>
   <si>
-    <t>准静止判定速度</t>
-  </si>
-  <si>
-    <t>v_static(m/s)</t>
-  </si>
-  <si>
-    <t>40/3.6 = 11.11m/s</t>
-  </si>
-  <si>
-    <t>事件类别</t>
-  </si>
-  <si>
-    <t>event_types</t>
-  </si>
-  <si>
-    <t>["crowd", "high_speed", "illegal_occupation", "incident_single_car", "incident", "intensive_speed_reduction", "low_speed", "spill"]</t>
-  </si>
-  <si>
-    <t>抛洒物检测</t>
-  </si>
-  <si>
-    <t>抛洒物处理容忍时间</t>
-  </si>
-  <si>
-    <t>t_tolerance(s)</t>
-  </si>
-  <si>
-    <t>300s</t>
-  </si>
-  <si>
-    <t>道路设计标准流量参考值</t>
-  </si>
-  <si>
-    <t>q_standard(v/h)</t>
-  </si>
-  <si>
-    <t>10000v/h</t>
-  </si>
-  <si>
-    <t>抛洒物置信度时间增长率</t>
-  </si>
-  <si>
-    <t>rate1(/frame)</t>
-  </si>
-  <si>
-    <t>1/(t_tolerance *FPS)</t>
-  </si>
-  <si>
-    <t>抛洒物置信度换道增长率</t>
-  </si>
-  <si>
-    <t>rate2(1)</t>
+    <t>超速持续时间</t>
+  </si>
+  <si>
+    <t>duration_high(s)</t>
+  </si>
+  <si>
+    <t>异常急刹</t>
+  </si>
+  <si>
+    <t>急刹加速度</t>
+  </si>
+  <si>
+    <t>a_intense(m/s^2)</t>
+  </si>
+  <si>
+    <t>3m/s^2</t>
+  </si>
+  <si>
+    <t>急刹持续时间</t>
+  </si>
+  <si>
+    <t>duration_intense(s)</t>
+  </si>
+  <si>
+    <t>1s</t>
   </si>
   <si>
     <t>事故检测</t>
@@ -173,6 +284,15 @@
     <t>5m(两车追尾距离等于1个车长)</t>
   </si>
   <si>
+    <t>车被撞停监测时间</t>
+  </si>
+  <si>
+    <t>t_supervise(s)</t>
+  </si>
+  <si>
+    <t>20s</t>
+  </si>
+  <si>
     <t>拥堵检测</t>
   </si>
   <si>
@@ -194,27 +314,6 @@
     <t>16.67m/s</t>
   </si>
   <si>
-    <t>异常急刹</t>
-  </si>
-  <si>
-    <t>急刹加速度</t>
-  </si>
-  <si>
-    <t>a_intense(m/s^2)</t>
-  </si>
-  <si>
-    <t>3m/s^2</t>
-  </si>
-  <si>
-    <t>急刹持续时间</t>
-  </si>
-  <si>
-    <t>duration_intense(s)</t>
-  </si>
-  <si>
-    <t>1s</t>
-  </si>
-  <si>
     <t>应急车道占用</t>
   </si>
   <si>
@@ -224,79 +323,10 @@
     <t>duration_occupation(s)</t>
   </si>
   <si>
-    <t>5s</t>
-  </si>
-  <si>
-    <t>停车</t>
-  </si>
-  <si>
-    <t>准静止持续时间</t>
-  </si>
-  <si>
-    <t>duration_static(s)</t>
-  </si>
-  <si>
-    <t>超速行驶</t>
-  </si>
-  <si>
-    <t>超速持续时间</t>
-  </si>
-  <si>
-    <t>duration_high(s)</t>
-  </si>
-  <si>
-    <t>低速行驶</t>
-  </si>
-  <si>
-    <t>低速持续时间</t>
-  </si>
-  <si>
-    <t>duration_low(s)</t>
-  </si>
-  <si>
-    <t>交通流计算参数</t>
-  </si>
-  <si>
-    <t>流量计算</t>
-  </si>
-  <si>
-    <t>交通量计算采样时间</t>
-  </si>
-  <si>
-    <t>q_cal_duration(s)</t>
-  </si>
-  <si>
-    <t>参数更新</t>
-  </si>
-  <si>
-    <t>计算间隔时间</t>
-  </si>
-  <si>
-    <t>cal_interval(s)</t>
-  </si>
-  <si>
-    <t>30s</t>
-  </si>
-  <si>
-    <t>预处理参数</t>
-  </si>
-  <si>
-    <t>轨迹补全</t>
-  </si>
-  <si>
-    <t>最大补全帧数</t>
-  </si>
-  <si>
-    <t>max_complete_frames</t>
-  </si>
-  <si>
-    <t>轨迹平滑</t>
-  </si>
-  <si>
-    <t>平滑指数</t>
-  </si>
-  <si>
-    <t>smooth_alpha</t>
+    <t>note</t>
+  </si>
+  <si>
+    <t>表中参数总数29，基础参数共28项，其中‘抛洒物检测--置信度时间增长率’这一参数在代码内运算。因此config中参数应为28项，需保持对应。</t>
   </si>
 </sst>
 </file>
@@ -687,7 +717,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -705,6 +735,43 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -834,7 +901,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -846,34 +913,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -958,7 +1025,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -971,10 +1038,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1519,10 +1595,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1549,7 +1625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" s="1" customFormat="1" ht="17.5" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1562,26 +1638,30 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="17.5" spans="1:5">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+    <row r="4" s="1" customFormat="1" ht="17.5" spans="1:5">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1593,8 +1673,8 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1606,51 +1686,51 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="5" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1661,118 +1741,126 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" ht="70" spans="1:5">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+    <row r="10" spans="1:5">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="C10" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
+      <c r="A11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E11" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" ht="56" spans="1:5">
+      <c r="A13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="D13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="C14" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="8">
+        <v>46</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="11">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="4"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="4" t="s">
         <v>55</v>
       </c>
@@ -1787,8 +1875,8 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="5" t="s">
         <v>59</v>
       </c>
@@ -1800,7 +1888,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="4"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="4" t="s">
         <v>62</v>
       </c>
@@ -1815,126 +1903,172 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="8"/>
+      <c r="B22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="5" t="s">
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="5" t="s">
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8"/>
+      <c r="B26" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="5" t="s">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4" t="s">
+      <c r="E27" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="5" t="s">
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="5">
-        <v>0.1</v>
-      </c>
+      <c r="D28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A30"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
fix: update v high param
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12080"/>
+    <workbookView windowWidth="13340" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
     <t>v_high(m/s)</t>
   </si>
   <si>
-    <t>120/3.6 = 33.33m/s</t>
+    <t>80/3.6 = 22.22m/s</t>
   </si>
   <si>
     <t>超速持续时间</t>
@@ -1597,8 +1597,8 @@
   <sheetPr/>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
fix: add new param
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13340" windowHeight="12080"/>
+    <workbookView windowWidth="25600" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
   <si>
     <t>参数类别</t>
   </si>
@@ -194,6 +194,15 @@
     <t>rate2(1)</t>
   </si>
   <si>
+    <t>横向速度判定数值(认定前方存在抛洒物)</t>
+  </si>
+  <si>
+    <t>v_lateral(m/s)</t>
+  </si>
+  <si>
+    <t>2/3.6=0.56m/s</t>
+  </si>
+  <si>
     <t>停车</t>
   </si>
   <si>
@@ -326,7 +335,7 @@
     <t>note</t>
   </si>
   <si>
-    <t>表中参数总数29，基础参数共28项，其中‘抛洒物检测--置信度时间增长率’这一参数在代码内运算。因此config中参数应为28项，需保持对应。</t>
+    <t>表中参数总数30，基础参数共29项，其中‘抛洒物检测--置信度时间增长率’这一参数在代码内运算。因此config中参数应为29项，需保持对应。</t>
   </si>
 </sst>
 </file>
@@ -1595,10 +1604,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1861,22 +1870,22 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8"/>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="C19" s="5" t="s">
         <v>59</v>
       </c>
@@ -1889,22 +1898,22 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8"/>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C21" s="5" t="s">
         <v>66</v>
       </c>
@@ -1912,14 +1921,12 @@
         <v>67</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8"/>
-      <c r="B22" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
         <v>69</v>
       </c>
@@ -1927,12 +1934,14 @@
         <v>70</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>72</v>
       </c>
@@ -1940,14 +1949,12 @@
         <v>73</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8"/>
-      <c r="B24" s="8" t="s">
-        <v>74</v>
-      </c>
+      <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
         <v>75</v>
       </c>
@@ -1955,12 +1962,14 @@
         <v>76</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
+      <c r="B25" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="C25" s="5" t="s">
         <v>78</v>
       </c>
@@ -1973,22 +1982,22 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8"/>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="C27" s="5" t="s">
         <v>85</v>
       </c>
@@ -2001,22 +2010,22 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8"/>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>92</v>
       </c>
@@ -2029,46 +2038,59 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8"/>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="5" t="s">
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A30"/>
+    <mergeCell ref="A13:A31"/>
     <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
fix: add param "spill warn frequency"
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
   <si>
     <t>参数类别</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>2/3.6=0.56m/s</t>
+  </si>
+  <si>
+    <t>抛洒物报警频率</t>
+  </si>
+  <si>
+    <t>spill_warn_frequecy(s)</t>
   </si>
   <si>
     <t>停车</t>
@@ -1034,7 +1040,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1069,6 +1075,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1604,10 +1613,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1883,214 +1892,227 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8"/>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>61</v>
+      <c r="E19" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8"/>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
+      <c r="B22" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="C22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="C24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8"/>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="C26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8"/>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8"/>
-      <c r="B28" s="7"/>
+      <c r="B28" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="C28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8"/>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="C30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8"/>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="5" t="s">
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A31"/>
+    <mergeCell ref="A13:A32"/>
     <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
fix: update param names
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -158,7 +158,7 @@
     <t>event_types</t>
   </si>
   <si>
-    <t>['spill','stop', 'low_speed', 'high_speed', 'emergency_break', 'incident', 'crowd', 'illegal_occupation']</t>
+    <t>["spill", "stop", "lowSpeed", "highSpeed", "emergencyBrake", "incident", "crowd", "illegalOccupation"]</t>
   </si>
   <si>
     <t>抛洒物检测</t>
@@ -1040,7 +1040,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1075,9 +1075,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1616,7 +1613,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1893,13 +1890,13 @@
     <row r="19" spans="1:5">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="5" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: update param name
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -56,13 +56,13 @@
     <t>是否重新标定(在clb存在情况下是否重来)</t>
   </si>
   <si>
-    <t>if_recalib</t>
+    <t>ifRecalib</t>
   </si>
   <si>
     <t>标定过程持续时间</t>
   </si>
   <si>
-    <t>calib_seconds(s)</t>
+    <t>calibSeconds(s)</t>
   </si>
   <si>
     <t>600s</t>
@@ -71,7 +71,7 @@
     <t>元胞分割距离</t>
   </si>
   <si>
-    <t>cell_len(m)</t>
+    <t>cellLen(m)</t>
   </si>
   <si>
     <t>50m</t>
@@ -80,13 +80,13 @@
     <t>合流元胞判定交通量</t>
   </si>
   <si>
-    <t>q_merge(v/h)</t>
+    <t>qMerge(v/h)</t>
   </si>
   <si>
     <t>普通车道宽度</t>
   </si>
   <si>
-    <t>lane_width(m)</t>
+    <t>laneWidth(m)</t>
   </si>
   <si>
     <t>3.75m</t>
@@ -95,7 +95,7 @@
     <t>应急车道宽度</t>
   </si>
   <si>
-    <t>emgc_width(m)</t>
+    <t>emgcWidth(m)</t>
   </si>
   <si>
     <t>3.5m</t>
@@ -110,7 +110,7 @@
     <t>交通量计算采样时间</t>
   </si>
   <si>
-    <t>q_cal_duration(s)</t>
+    <t>qCalDuration(s)</t>
   </si>
   <si>
     <t>300s</t>
@@ -122,7 +122,7 @@
     <t>计算间隔时间</t>
   </si>
   <si>
-    <t>cal_interval(s)</t>
+    <t>calInterval(s)</t>
   </si>
   <si>
     <t>30s</t>
@@ -137,7 +137,7 @@
     <t>最大补全帧数</t>
   </si>
   <si>
-    <t>max_complete_frames</t>
+    <t>maxCompleteFrames</t>
   </si>
   <si>
     <t>轨迹平滑</t>
@@ -146,7 +146,7 @@
     <t>平滑指数</t>
   </si>
   <si>
-    <t>smooth_alpha</t>
+    <t>smoothAlpha</t>
   </si>
   <si>
     <t>事件检测</t>
@@ -155,7 +155,7 @@
     <t>事件类别</t>
   </si>
   <si>
-    <t>event_types</t>
+    <t>eventTypes</t>
   </si>
   <si>
     <t>["spill", "stop", "lowSpeed", "highSpeed", "emergencyBrake", "incident", "crowd", "illegalOccupation"]</t>
@@ -167,13 +167,13 @@
     <t>抛洒物处理容忍时间</t>
   </si>
   <si>
-    <t>t_tolerance(s)</t>
+    <t>tTolerance(s)</t>
   </si>
   <si>
     <t>道路设计标准流量参考值</t>
   </si>
   <si>
-    <t>q_standard(v/h)</t>
+    <t>qStandard(v/h)</t>
   </si>
   <si>
     <t>10000v/h</t>
@@ -197,7 +197,7 @@
     <t>横向速度判定数值(认定前方存在抛洒物)</t>
   </si>
   <si>
-    <t>v_lateral(m/s)</t>
+    <t>vLateral(m/s)</t>
   </si>
   <si>
     <t>2/3.6=0.56m/s</t>
@@ -206,7 +206,7 @@
     <t>抛洒物报警频率</t>
   </si>
   <si>
-    <t>spill_warn_frequecy(s)</t>
+    <t>spillWarnFrequecy(s)</t>
   </si>
   <si>
     <t>停车</t>
@@ -215,7 +215,7 @@
     <t>准静止判定速度</t>
   </si>
   <si>
-    <t>v_static(m/s)</t>
+    <t>vStop(m/s)</t>
   </si>
   <si>
     <t>3.6/3.6 = 1m/s</t>
@@ -224,7 +224,7 @@
     <t>准静止持续时间</t>
   </si>
   <si>
-    <t>duration_static(s)</t>
+    <t>durationStop(s)</t>
   </si>
   <si>
     <t>5s</t>
@@ -236,7 +236,7 @@
     <t>低速判定速度</t>
   </si>
   <si>
-    <t>v_low(m/s)</t>
+    <t>vLow(m/s)</t>
   </si>
   <si>
     <t>10/3.6 = 2.778m/s</t>
@@ -245,7 +245,7 @@
     <t>低速持续时间</t>
   </si>
   <si>
-    <t>duration_low(s)</t>
+    <t>durationLow(s)</t>
   </si>
   <si>
     <t>超速行驶</t>
@@ -254,7 +254,7 @@
     <t>高速判定速度</t>
   </si>
   <si>
-    <t>v_high(m/s)</t>
+    <t>vHigh(m/s)</t>
   </si>
   <si>
     <t>80/3.6 = 22.22m/s</t>
@@ -263,7 +263,7 @@
     <t>超速持续时间</t>
   </si>
   <si>
-    <t>duration_high(s)</t>
+    <t>durationHigh(s)</t>
   </si>
   <si>
     <t>异常急刹</t>
@@ -272,7 +272,7 @@
     <t>急刹加速度</t>
   </si>
   <si>
-    <t>a_intense(m/s^2)</t>
+    <t>aIntense(m/s^2)</t>
   </si>
   <si>
     <t>3m/s^2</t>
@@ -281,7 +281,7 @@
     <t>急刹持续时间</t>
   </si>
   <si>
-    <t>duration_intense(s)</t>
+    <t>durationIntense(s)</t>
   </si>
   <si>
     <t>1s</t>
@@ -293,7 +293,7 @@
     <t>接触距离</t>
   </si>
   <si>
-    <t>d_touch(m)</t>
+    <t>dTouch(m)</t>
   </si>
   <si>
     <t>5m(两车追尾距离等于1个车长)</t>
@@ -302,7 +302,7 @@
     <t>车被撞停监测时间</t>
   </si>
   <si>
-    <t>t_supervise(s)</t>
+    <t>tSupervise(s)</t>
   </si>
   <si>
     <t>20s</t>
@@ -314,7 +314,7 @@
     <t>拥堵密度</t>
   </si>
   <si>
-    <t>density_crowd(pcu/km/ln)</t>
+    <t>densityCrowd(pcu/km/ln)</t>
   </si>
   <si>
     <t>18pcu/km/ln</t>
@@ -323,7 +323,7 @@
     <t>拥堵速度</t>
   </si>
   <si>
-    <t>v_crowd(m/s)</t>
+    <t>vCrowd(m/s)</t>
   </si>
   <si>
     <t>16.67m/s</t>
@@ -335,7 +335,7 @@
     <t>占用持续时间</t>
   </si>
   <si>
-    <t>duration_occupation(s)</t>
+    <t>durationOccupation(s)</t>
   </si>
   <si>
     <t>note</t>
@@ -1613,7 +1613,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
fix: rename emergency as emgc
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -272,7 +272,7 @@
     <t>急刹加速度</t>
   </si>
   <si>
-    <t>aIntense(m/s^2)</t>
+    <t>aEmgcBrake(m/s^2)</t>
   </si>
   <si>
     <t>3m/s^2</t>
@@ -281,7 +281,7 @@
     <t>急刹持续时间</t>
   </si>
   <si>
-    <t>durationIntense(s)</t>
+    <t>durationEmgcBrake(s)</t>
   </si>
   <si>
     <t>1s</t>
@@ -1613,7 +1613,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
fix: adjust time unit for complete from 'frames' to 'time'
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
   <si>
     <t>参数类别</t>
   </si>
@@ -134,10 +134,13 @@
     <t>轨迹补全</t>
   </si>
   <si>
-    <t>最大补全帧数</t>
-  </si>
-  <si>
-    <t>maxCompleteFrames</t>
+    <t>最大补全时间</t>
+  </si>
+  <si>
+    <t>maxCompleteTime(s)</t>
+  </si>
+  <si>
+    <t>2s</t>
   </si>
   <si>
     <t>轨迹平滑</t>
@@ -1613,7 +1616,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1784,20 +1787,20 @@
       <c r="D11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="5">
-        <v>20</v>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="5">
         <v>0.1</v>
@@ -1805,31 +1808,31 @@
     </row>
     <row r="13" ht="56" spans="1:5">
       <c r="A13" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="8"/>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>28</v>
@@ -1839,36 +1842,36 @@
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E17" s="11">
         <v>0.1</v>
@@ -1878,23 +1881,23 @@
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>28</v>
@@ -1903,192 +1906,192 @@
     <row r="20" spans="1:5">
       <c r="A20" s="8"/>
       <c r="B20" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8"/>
       <c r="B22" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8"/>
       <c r="B24" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8"/>
       <c r="B26" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8"/>
       <c r="B28" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8"/>
       <c r="B30" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>

</xml_diff>

<commit_message>
fix: update param value
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
   <si>
     <t>参数类别</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>rate2(1)</t>
+  </si>
+  <si>
+    <t>0.0017(设定某cell有10辆车换道, 判定前方有spill。假定每辆车换道耗时3s, 对应60帧数据,期间车辆横向速度大于限值,以rate2增长,则rate2=1/10/60=0.0017)</t>
   </si>
   <si>
     <t>横向速度判定数值(认定前方存在抛洒物)</t>
@@ -1078,7 +1081,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1616,7 +1619,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1864,7 +1867,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" ht="56" spans="1:5">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="5" t="s">
@@ -1873,31 +1876,31 @@
       <c r="D17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="11">
-        <v>0.1</v>
+      <c r="E17" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>28</v>
@@ -1906,192 +1909,192 @@
     <row r="20" spans="1:5">
       <c r="A20" s="8"/>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8"/>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8"/>
       <c r="B24" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8"/>
       <c r="B26" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8"/>
       <c r="B28" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8"/>
       <c r="B30" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>

</xml_diff>

<commit_message>
fix: update config parameters
</commit_message>
<xml_diff>
--- a/docs/parameter.xlsx
+++ b/docs/parameter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12080"/>
+    <workbookView windowWidth="20850" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
     <t>rate2(1)</t>
   </si>
   <si>
-    <t>0.0017(设定某cell有10辆车换道, 判定前方有spill。假定每辆车换道耗时3s, 对应60帧数据,期间车辆横向速度大于限值,以rate2增长,则rate2=1/10/60=0.0017)</t>
+    <t>0.0017(设定某cell有10辆车换道, 判定前方有spill。假定每辆车换道耗时5s, 对应100帧数据,期间车辆横向速度大于限值,以rate2增长,则rate2=0.5/10/100=0.0005)</t>
   </si>
   <si>
     <t>横向速度判定数值(认定前方存在抛洒物)</t>
@@ -1619,7 +1619,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="4"/>

</xml_diff>